<commit_message>
Generate List of Order
The list of order when there is Musical chairs mechanism
</commit_message>
<xml_diff>
--- a/Order.xlsx
+++ b/Order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OASYS\Commencement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED0393F-869D-42FE-98FA-58F6CA32C0EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508D8998-1C25-4153-9839-EB2211D14C82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29190" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{33855BC1-CE2C-4067-AA61-0A6F44B94D8D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{33855BC1-CE2C-4067-AA61-0A6F44B94D8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Morning Order" sheetId="1" r:id="rId1"/>
@@ -918,7 +918,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
@@ -1080,7 +1080,7 @@
         <v>43</v>
       </c>
       <c r="C9" s="14">
-        <v>0</v>
+        <v>303</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="37" t="s">
@@ -1098,7 +1098,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="14">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="37" t="s">
@@ -1116,7 +1116,7 @@
         <v>45</v>
       </c>
       <c r="C11" s="14">
-        <v>0</v>
+        <v>411</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="37" t="s">
@@ -1134,7 +1134,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="14">
-        <v>0</v>
+        <v>221</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="37" t="s">
@@ -1152,7 +1152,7 @@
         <v>47</v>
       </c>
       <c r="C13" s="14">
-        <v>0</v>
+        <v>305</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="37" t="s">

</xml_diff>

<commit_message>
finish list and fill template
</commit_message>
<xml_diff>
--- a/Order.xlsx
+++ b/Order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanarutboonyung/Desktop/Works/OASYS/Commencement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3AD5C5-1B7C-B64E-8229-4E246ADD05A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794EB378-8358-1842-8BA0-DF08EF274038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19760" xr2:uid="{33855BC1-CE2C-4067-AA61-0A6F44B94D8D}"/>
   </bookViews>
@@ -921,7 +921,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>